<commit_message>
lots of work figuring out vesc and finally think things are working.
</commit_message>
<xml_diff>
--- a/test rig/bldc comparison.xlsx
+++ b/test rig/bldc comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t xml:space="preserve">Motor</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux Linkage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observer Gain</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -122,8 +128,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -131,6 +138,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,6 +161,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +237,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -251,10 +264,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -267,8 +280,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="13" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,19 +320,25 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>54</v>
@@ -326,41 +347,49 @@
         <v>170</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>785</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>14</v>
       </c>
       <c r="K2" s="0"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J2 * PI() * D2)) * 1000</f>
+        <v>4.63301592791422</v>
+      </c>
+      <c r="M2" s="8" t="n">
+        <f aca="false">1000 / (L2^2)</f>
+        <v>46.5878226412755</v>
+      </c>
+      <c r="N2" s="9"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>50</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>300</v>
@@ -372,13 +401,13 @@
         <v>310</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J3" s="7" t="n">
         <v>28</v>
@@ -386,19 +415,27 @@
       <c r="K3" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
+      <c r="L3" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J3 * PI() * D3)) * 1000</f>
+        <v>1.31268784624236</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <f aca="false">1000 / (L3^2)</f>
+        <v>580.332738784054</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>160</v>
@@ -410,13 +447,13 @@
         <v>500</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>14</v>
@@ -424,10 +461,18 @@
       <c r="K4" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="L4" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J4 * PI() * D4)) * 1000</f>
+        <v>4.92257942340886</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <f aca="false">1000 / (L4^2)</f>
+        <v>41.2681058690883</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>99</v>
@@ -442,13 +487,13 @@
         <v>680</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>28</v>
@@ -456,10 +501,18 @@
       <c r="K5" s="1" t="n">
         <v>45</v>
       </c>
+      <c r="L5" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J5 * PI() * D5)) * 1000</f>
+        <v>2.8129025276622</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <f aca="false">1000 / (L5^2)</f>
+        <v>126.383574224083</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>195</v>
@@ -474,10 +527,10 @@
         <v>1400</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>8</v>
@@ -485,13 +538,21 @@
       <c r="K6" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>24</v>
+      <c r="L6" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J6 * PI() * D6)) * 1000</f>
+        <v>10.6024787581114</v>
+      </c>
+      <c r="M6" s="8" t="n">
+        <f aca="false">1000 / (L6^2)</f>
+        <v>8.8958034335152</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>459</v>
@@ -506,10 +567,10 @@
         <v>3000</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>6</v>
@@ -517,33 +578,41 @@
       <c r="K7" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>26</v>
+      <c r="L7" s="8" t="n">
+        <f aca="false">(60/(SQRT(3) * J7 * PI() * D7)) * 1000</f>
+        <v>18.3776298473931</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <f aca="false">1000 / (L7^2)</f>
+        <v>2.96088132032681</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on the stats script a bit
</commit_message>
<xml_diff>
--- a/test rig/bldc comparison.xlsx
+++ b/test rig/bldc comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t xml:space="preserve">Motor</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">Write an arduino / raspberry pi script to record speed, wattage, and drag from strain gauge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulas from: https://vesc-project.com/node/52</t>
   </si>
 </sst>
 </file>
@@ -264,10 +267,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,8 +283,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="1" width="9.14"/>
   </cols>
@@ -615,7 +618,15 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A20" r:id="rId1" display="https://vesc-project.com/node/52"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>